<commit_message>
Updated contents of coursework code and results
</commit_message>
<xml_diff>
--- a/finals/task3/task3_1/joint_errors.xlsx
+++ b/finals/task3/task3_1/joint_errors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23250" windowHeight="20310" activeTab="1"/>
+    <workbookView windowWidth="31770" windowHeight="20370" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1155,8 +1155,8 @@
   <sheetPr/>
   <dimension ref="A1:K241"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A192" workbookViewId="0">
-      <selection activeCell="A162" sqref="A162:E241"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="E194" sqref="E194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -5100,15 +5100,14 @@
   <sheetPr/>
   <dimension ref="A1:P81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="2" width="4.2" customWidth="1"/>
-    <col min="3" max="4" width="11.0666666666667"/>
-    <col min="5" max="5" width="8.53333333333333" customWidth="1"/>
+    <col min="3" max="5" width="19.92" customWidth="1"/>
     <col min="7" max="8" width="15.8666666666667" customWidth="1"/>
     <col min="9" max="9" width="12.1333333333333"/>
     <col min="10" max="10" width="10.3333333333333"/>
@@ -5420,7 +5419,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="12" ht="17.25" spans="1:13">
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -5587,7 +5586,6 @@
       <c r="C17" t="s">
         <v>6</v>
       </c>
-      <c r="D17"/>
       <c r="F17" s="7" t="s">
         <v>4</v>
       </c>
@@ -5868,7 +5866,6 @@
       <c r="H28" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I28"/>
       <c r="J28" s="1" t="s">
         <v>2</v>
       </c>
@@ -6000,7 +5997,7 @@
         <v>3</v>
       </c>
       <c r="G31" s="2">
-        <f t="shared" ref="G30:G35" si="1">AVERAGE(D4,D12,D20,D28,D36,D44,D52,D60,D68,D76)</f>
+        <f>AVERAGE(D4,D12,D20,D28,D36,D44,D52,D60,D68,D76)</f>
         <v>0.0666496324640011</v>
       </c>
       <c r="H31" s="2">
@@ -6046,7 +6043,7 @@
         <v>4</v>
       </c>
       <c r="G32" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="G30:G35" si="1">AVERAGE(D5,D13,D21,D29,D37,D45,D53,D61,D69,D77)</f>
         <v>0.842501796317161</v>
       </c>
       <c r="H32" s="2">
@@ -6082,8 +6079,6 @@
       <c r="C33" t="s">
         <v>6</v>
       </c>
-      <c r="D33"/>
-      <c r="E33"/>
       <c r="F33">
         <v>5</v>
       </c>
@@ -6379,7 +6374,6 @@
       <c r="C41" t="s">
         <v>6</v>
       </c>
-      <c r="D41"/>
       <c r="F41">
         <v>4</v>
       </c>
@@ -7582,7 +7576,7 @@
         <v>4</v>
       </c>
       <c r="G18" s="2">
-        <f>AVERAGE(D5,D13,D21,D29,D37,D45,D53,D61,D69,D77)</f>
+        <f t="shared" si="0"/>
         <v>2.96979559234956</v>
       </c>
       <c r="H18" s="2">

</xml_diff>